<commit_message>
adding spefications for exterior blinds
</commit_message>
<xml_diff>
--- a/data/material.xlsx
+++ b/data/material.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrenis\gitprojects\BuildME\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A2D9019-C0E5-4C9A-A2BB-A5DEB43DF561}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCCA4375-3174-4A1A-8A44-D65A2BA08DD7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{F14F42AE-B2B5-F34E-80E7-10F24B944563}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
   <si>
     <t>Bldg_paper_felt</t>
   </si>
@@ -104,6 +104,9 @@
   </si>
   <si>
     <t>ext_blind_test</t>
+  </si>
+  <si>
+    <t>ext_blind</t>
   </si>
 </sst>
 </file>
@@ -472,10 +475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E70C4D75-A999-1F4A-8C48-1C4FDC3CB665}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15"/>
@@ -675,6 +678,20 @@
       </c>
       <c r="E12" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Archetypes are implemented to BuildME
All of the archetypes are converted by using Ideal Loads converter, IDF converter and by Kamila's FC construction method.

There are still some missing features but these are not mandatory to address, these are:
-Airthightness Values across different standards (can be edited in replace.xlsx)
-Other RES scenarios than RES0
-Material specific thickness values ( right now I only added a placeholder value for all of the new ones, it can be accessed in material.xlsx and changed with realistic values)
</commit_message>
<xml_diff>
--- a/data/material.xlsx
+++ b/data/material.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrenis\gitprojects\BuildME\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sahina\PycharmProjects\Kamila\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCCA4375-3174-4A1A-8A44-D65A2BA08DD7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A12EEDEB-AFE0-4BA9-9ACA-8ED29460F6A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{F14F42AE-B2B5-F34E-80E7-10F24B944563}"/>
+    <workbookView xWindow="95880" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{F14F42AE-B2B5-F34E-80E7-10F24B944563}"/>
   </bookViews>
   <sheets>
     <sheet name="properties" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="98">
   <si>
     <t>Bldg_paper_felt</t>
   </si>
@@ -107,6 +110,225 @@
   </si>
   <si>
     <t>ext_blind</t>
+  </si>
+  <si>
+    <t>Opaque Door panel_con-efficient-RES0</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>Overhead Door_con Panel-efficient-RES0</t>
+  </si>
+  <si>
+    <t>CP02 CARPET PAD-efficient-RES0</t>
+  </si>
+  <si>
+    <t>Air_Wall_Material-efficient-RES0</t>
+  </si>
+  <si>
+    <t>Nonres_Roof_Insulation-efficient-RES0</t>
+  </si>
+  <si>
+    <t>Res_Roof_Insulation-efficient-RES0</t>
+  </si>
+  <si>
+    <t>Semiheated_Roof_Insulation-efficient-RES0</t>
+  </si>
+  <si>
+    <t>Nonres_Exterior_Wall_Insulation-efficient-RES0</t>
+  </si>
+  <si>
+    <t>Res_Exterior_Wall_Insulation-efficient-RES0</t>
+  </si>
+  <si>
+    <t>Semiheated_Exterior_Wall_Insulation-efficient-RES0</t>
+  </si>
+  <si>
+    <t>Nonres_Floor_Insulation-efficient-RES0</t>
+  </si>
+  <si>
+    <t>Res_Floor_Insulation-efficient-RES0</t>
+  </si>
+  <si>
+    <t>Semiheated_Floor_Insulation-efficient-RES0</t>
+  </si>
+  <si>
+    <t>Std Opaque Door Panel-efficient-RES0</t>
+  </si>
+  <si>
+    <t>Opaque Door panel_con-non-standard-RES0</t>
+  </si>
+  <si>
+    <t>Overhead Door_con Panel-non-standard-RES0</t>
+  </si>
+  <si>
+    <t>CP02 CARPET PAD-non-standard-RES0</t>
+  </si>
+  <si>
+    <t>Air_Wall_Material-non-standard-RES0</t>
+  </si>
+  <si>
+    <t>Nonres_Roof_Insulation-non-standard-RES0</t>
+  </si>
+  <si>
+    <t>Res_Roof_Insulation-non-standard-RES0</t>
+  </si>
+  <si>
+    <t>Semiheated_Roof_Insulation-non-standard-RES0</t>
+  </si>
+  <si>
+    <t>Nonres_Exterior_Wall_Insulation-non-standard-RES0</t>
+  </si>
+  <si>
+    <t>Res_Exterior_Wall_Insulation-non-standard-RES0</t>
+  </si>
+  <si>
+    <t>Semiheated_Exterior_Wall_Insulation-non-standard-RES0</t>
+  </si>
+  <si>
+    <t>Nonres_Floor_Insulation-non-standard-RES0</t>
+  </si>
+  <si>
+    <t>Res_Floor_Insulation-non-standard-RES0</t>
+  </si>
+  <si>
+    <t>Semiheated_Floor_Insulation-non-standard-RES0</t>
+  </si>
+  <si>
+    <t>Std Opaque Door Panel-non-standard-RES0</t>
+  </si>
+  <si>
+    <t>Opaque Door panel_con-standard-RES0</t>
+  </si>
+  <si>
+    <t>Overhead Door_con Panel-standard-RES0</t>
+  </si>
+  <si>
+    <t>CP02 CARPET PAD-standard-RES0</t>
+  </si>
+  <si>
+    <t>Air_Wall_Material-standard-RES0</t>
+  </si>
+  <si>
+    <t>Nonres_Roof_Insulation-standard-RES0</t>
+  </si>
+  <si>
+    <t>Res_Roof_Insulation-standard-RES0</t>
+  </si>
+  <si>
+    <t>Semiheated_Roof_Insulation-standard-RES0</t>
+  </si>
+  <si>
+    <t>Nonres_Exterior_Wall_Insulation-standard-RES0</t>
+  </si>
+  <si>
+    <t>Res_Exterior_Wall_Insulation-standard-RES0</t>
+  </si>
+  <si>
+    <t>Semiheated_Exterior_Wall_Insulation-standard-RES0</t>
+  </si>
+  <si>
+    <t>Nonres_Floor_Insulation-standard-RES0</t>
+  </si>
+  <si>
+    <t>Res_Floor_Insulation-standard-RES0</t>
+  </si>
+  <si>
+    <t>Semiheated_Floor_Insulation-standard-RES0</t>
+  </si>
+  <si>
+    <t>Std Opaque Door Panel-standard-RES0</t>
+  </si>
+  <si>
+    <t>Opaque Door panel_con-ZEB-RES0</t>
+  </si>
+  <si>
+    <t>Overhead Door_con Panel-ZEB-RES0</t>
+  </si>
+  <si>
+    <t>CP02 CARPET PAD-ZEB-RES0</t>
+  </si>
+  <si>
+    <t>Air_Wall_Material-ZEB-RES0</t>
+  </si>
+  <si>
+    <t>Nonres_Roof_Insulation-ZEB-RES0</t>
+  </si>
+  <si>
+    <t>Res_Roof_Insulation-ZEB-RES0</t>
+  </si>
+  <si>
+    <t>Semiheated_Roof_Insulation-ZEB-RES0</t>
+  </si>
+  <si>
+    <t>Nonres_Exterior_Wall_Insulation-ZEB-RES0</t>
+  </si>
+  <si>
+    <t>Res_Exterior_Wall_Insulation-ZEB-RES0</t>
+  </si>
+  <si>
+    <t>Semiheated_Exterior_Wall_Insulation-ZEB-RES0</t>
+  </si>
+  <si>
+    <t>Nonres_Floor_Insulation-ZEB-RES0</t>
+  </si>
+  <si>
+    <t>Res_Floor_Insulation-ZEB-RES0</t>
+  </si>
+  <si>
+    <t>Semiheated_Floor_Insulation-ZEB-RES0</t>
+  </si>
+  <si>
+    <t>Std Opaque Door Panel-ZEB-RES0</t>
+  </si>
+  <si>
+    <t>Glazing Layer-efficient-RES0</t>
+  </si>
+  <si>
+    <t>Residential Window Glazing Layer-efficient-RES0</t>
+  </si>
+  <si>
+    <t>Glazing Layer-non-standard-RES0</t>
+  </si>
+  <si>
+    <t>Residential Window Glazing Layer-non-standard-RES0</t>
+  </si>
+  <si>
+    <t>Glazing Layer-standard-RES0</t>
+  </si>
+  <si>
+    <t>Residential Window Glazing Layer-standard-RES0</t>
+  </si>
+  <si>
+    <t>Glazing Layer-ZEB-RES0</t>
+  </si>
+  <si>
+    <t>Residential Window Glazing Layer-ZEB-RES0</t>
+  </si>
+  <si>
+    <t>Nonres Window Glazing Layer-efficient-RES0</t>
+  </si>
+  <si>
+    <t>Nonres Skylight Glazing Layer-efficient-RES0</t>
+  </si>
+  <si>
+    <t>Nonres Window Glazing Layer-non-standard-RES0</t>
+  </si>
+  <si>
+    <t>Nonres Skylight Glazing Layer-non-standard-RES0</t>
+  </si>
+  <si>
+    <t>Nonres Window Glazing Layer-standard-RES0</t>
+  </si>
+  <si>
+    <t>Nonres Skylight Glazing Layer-standard-RES0</t>
+  </si>
+  <si>
+    <t>Nonres Window Glazing Layer-ZEB-RES0</t>
+  </si>
+  <si>
+    <t>Nonres Skylight Glazing Layer-ZEB-RES0</t>
   </si>
 </sst>
 </file>
@@ -475,19 +697,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E70C4D75-A999-1F4A-8C48-1C4FDC3CB665}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="A69" sqref="A69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15.25"/>
   <cols>
-    <col min="1" max="1" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="47.0703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75">
+    <row r="1" spans="1:5" ht="15.5">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -555,7 +777,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" ht="15.5">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -570,7 +792,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" ht="15.5">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -585,7 +807,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" ht="15.5">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -600,7 +822,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" ht="15.5">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -632,7 +854,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" ht="15.5">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -649,7 +871,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" ht="15.5">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -692,6 +914,1230 @@
       </c>
       <c r="D13">
         <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14">
+        <v>2500</v>
+      </c>
+      <c r="C14">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D14">
+        <v>0.9</v>
+      </c>
+      <c r="E14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15">
+        <v>2500</v>
+      </c>
+      <c r="C15">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D15">
+        <v>0.9</v>
+      </c>
+      <c r="E15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16">
+        <v>2500</v>
+      </c>
+      <c r="C16">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D16">
+        <v>0.9</v>
+      </c>
+      <c r="E16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17">
+        <v>2500</v>
+      </c>
+      <c r="C17">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D17">
+        <v>0.9</v>
+      </c>
+      <c r="E17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18">
+        <v>2500</v>
+      </c>
+      <c r="C18">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D18">
+        <v>0.9</v>
+      </c>
+      <c r="E18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19">
+        <v>2500</v>
+      </c>
+      <c r="C19">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D19">
+        <v>0.9</v>
+      </c>
+      <c r="E19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20">
+        <v>2500</v>
+      </c>
+      <c r="C20">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D20">
+        <v>0.9</v>
+      </c>
+      <c r="E20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21">
+        <v>2500</v>
+      </c>
+      <c r="C21">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D21">
+        <v>0.9</v>
+      </c>
+      <c r="E21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22">
+        <v>2500</v>
+      </c>
+      <c r="C22">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D22">
+        <v>0.9</v>
+      </c>
+      <c r="E22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23">
+        <v>2500</v>
+      </c>
+      <c r="C23">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D23">
+        <v>0.9</v>
+      </c>
+      <c r="E23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24">
+        <v>2500</v>
+      </c>
+      <c r="C24">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D24">
+        <v>0.9</v>
+      </c>
+      <c r="E24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25">
+        <v>2500</v>
+      </c>
+      <c r="C25">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D25">
+        <v>0.9</v>
+      </c>
+      <c r="E25" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26">
+        <v>2500</v>
+      </c>
+      <c r="C26">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D26">
+        <v>0.9</v>
+      </c>
+      <c r="E26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27">
+        <v>2500</v>
+      </c>
+      <c r="C27">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D27">
+        <v>0.9</v>
+      </c>
+      <c r="E27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28">
+        <v>2500</v>
+      </c>
+      <c r="C28">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D28">
+        <v>0.9</v>
+      </c>
+      <c r="E28" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29">
+        <v>2500</v>
+      </c>
+      <c r="C29">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D29">
+        <v>0.9</v>
+      </c>
+      <c r="E29" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" t="s">
+        <v>42</v>
+      </c>
+      <c r="B30">
+        <v>2500</v>
+      </c>
+      <c r="C30">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D30">
+        <v>0.9</v>
+      </c>
+      <c r="E30" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31">
+        <v>2500</v>
+      </c>
+      <c r="C31">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D31">
+        <v>0.9</v>
+      </c>
+      <c r="E31" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" t="s">
+        <v>44</v>
+      </c>
+      <c r="B32">
+        <v>2500</v>
+      </c>
+      <c r="C32">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D32">
+        <v>0.9</v>
+      </c>
+      <c r="E32" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" t="s">
+        <v>45</v>
+      </c>
+      <c r="B33">
+        <v>2500</v>
+      </c>
+      <c r="C33">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D33">
+        <v>0.9</v>
+      </c>
+      <c r="E33" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" t="s">
+        <v>46</v>
+      </c>
+      <c r="B34">
+        <v>2500</v>
+      </c>
+      <c r="C34">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D34">
+        <v>0.9</v>
+      </c>
+      <c r="E34" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" t="s">
+        <v>47</v>
+      </c>
+      <c r="B35">
+        <v>2500</v>
+      </c>
+      <c r="C35">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D35">
+        <v>0.9</v>
+      </c>
+      <c r="E35" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" t="s">
+        <v>48</v>
+      </c>
+      <c r="B36">
+        <v>2500</v>
+      </c>
+      <c r="C36">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D36">
+        <v>0.9</v>
+      </c>
+      <c r="E36" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" t="s">
+        <v>49</v>
+      </c>
+      <c r="B37">
+        <v>2500</v>
+      </c>
+      <c r="C37">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D37">
+        <v>0.9</v>
+      </c>
+      <c r="E37" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" t="s">
+        <v>50</v>
+      </c>
+      <c r="B38">
+        <v>2500</v>
+      </c>
+      <c r="C38">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D38">
+        <v>0.9</v>
+      </c>
+      <c r="E38" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" t="s">
+        <v>51</v>
+      </c>
+      <c r="B39">
+        <v>2500</v>
+      </c>
+      <c r="C39">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D39">
+        <v>0.9</v>
+      </c>
+      <c r="E39" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" t="s">
+        <v>52</v>
+      </c>
+      <c r="B40">
+        <v>2500</v>
+      </c>
+      <c r="C40">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D40">
+        <v>0.9</v>
+      </c>
+      <c r="E40" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" t="s">
+        <v>53</v>
+      </c>
+      <c r="B41">
+        <v>2500</v>
+      </c>
+      <c r="C41">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D41">
+        <v>0.9</v>
+      </c>
+      <c r="E41" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" t="s">
+        <v>54</v>
+      </c>
+      <c r="B42">
+        <v>2500</v>
+      </c>
+      <c r="C42">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D42">
+        <v>0.9</v>
+      </c>
+      <c r="E42" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" t="s">
+        <v>55</v>
+      </c>
+      <c r="B43">
+        <v>2500</v>
+      </c>
+      <c r="C43">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D43">
+        <v>0.9</v>
+      </c>
+      <c r="E43" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" t="s">
+        <v>56</v>
+      </c>
+      <c r="B44">
+        <v>2500</v>
+      </c>
+      <c r="C44">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D44">
+        <v>0.9</v>
+      </c>
+      <c r="E44" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" t="s">
+        <v>57</v>
+      </c>
+      <c r="B45">
+        <v>2500</v>
+      </c>
+      <c r="C45">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D45">
+        <v>0.9</v>
+      </c>
+      <c r="E45" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" t="s">
+        <v>58</v>
+      </c>
+      <c r="B46">
+        <v>2500</v>
+      </c>
+      <c r="C46">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D46">
+        <v>0.9</v>
+      </c>
+      <c r="E46" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" t="s">
+        <v>59</v>
+      </c>
+      <c r="B47">
+        <v>2500</v>
+      </c>
+      <c r="C47">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D47">
+        <v>0.9</v>
+      </c>
+      <c r="E47" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" t="s">
+        <v>60</v>
+      </c>
+      <c r="B48">
+        <v>2500</v>
+      </c>
+      <c r="C48">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D48">
+        <v>0.9</v>
+      </c>
+      <c r="E48" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" t="s">
+        <v>61</v>
+      </c>
+      <c r="B49">
+        <v>2500</v>
+      </c>
+      <c r="C49">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D49">
+        <v>0.9</v>
+      </c>
+      <c r="E49" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" t="s">
+        <v>62</v>
+      </c>
+      <c r="B50">
+        <v>2500</v>
+      </c>
+      <c r="C50">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D50">
+        <v>0.9</v>
+      </c>
+      <c r="E50" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" t="s">
+        <v>63</v>
+      </c>
+      <c r="B51">
+        <v>2500</v>
+      </c>
+      <c r="C51">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D51">
+        <v>0.9</v>
+      </c>
+      <c r="E51" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" t="s">
+        <v>64</v>
+      </c>
+      <c r="B52">
+        <v>2500</v>
+      </c>
+      <c r="C52">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D52">
+        <v>0.9</v>
+      </c>
+      <c r="E52" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" t="s">
+        <v>65</v>
+      </c>
+      <c r="B53">
+        <v>2500</v>
+      </c>
+      <c r="C53">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D53">
+        <v>0.9</v>
+      </c>
+      <c r="E53" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" t="s">
+        <v>66</v>
+      </c>
+      <c r="B54">
+        <v>2500</v>
+      </c>
+      <c r="C54">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D54">
+        <v>0.9</v>
+      </c>
+      <c r="E54" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" t="s">
+        <v>67</v>
+      </c>
+      <c r="B55">
+        <v>2500</v>
+      </c>
+      <c r="C55">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D55">
+        <v>0.9</v>
+      </c>
+      <c r="E55" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" t="s">
+        <v>68</v>
+      </c>
+      <c r="B56">
+        <v>2500</v>
+      </c>
+      <c r="C56">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D56">
+        <v>0.9</v>
+      </c>
+      <c r="E56" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" t="s">
+        <v>69</v>
+      </c>
+      <c r="B57">
+        <v>2500</v>
+      </c>
+      <c r="C57">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D57">
+        <v>0.9</v>
+      </c>
+      <c r="E57" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" t="s">
+        <v>70</v>
+      </c>
+      <c r="B58">
+        <v>2500</v>
+      </c>
+      <c r="C58">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D58">
+        <v>0.9</v>
+      </c>
+      <c r="E58" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" t="s">
+        <v>71</v>
+      </c>
+      <c r="B59">
+        <v>2500</v>
+      </c>
+      <c r="C59">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D59">
+        <v>0.9</v>
+      </c>
+      <c r="E59" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" t="s">
+        <v>72</v>
+      </c>
+      <c r="B60">
+        <v>2500</v>
+      </c>
+      <c r="C60">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D60">
+        <v>0.9</v>
+      </c>
+      <c r="E60" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" t="s">
+        <v>73</v>
+      </c>
+      <c r="B61">
+        <v>2500</v>
+      </c>
+      <c r="C61">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D61">
+        <v>0.9</v>
+      </c>
+      <c r="E61" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" t="s">
+        <v>74</v>
+      </c>
+      <c r="B62">
+        <v>2500</v>
+      </c>
+      <c r="C62">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D62">
+        <v>0.9</v>
+      </c>
+      <c r="E62" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" t="s">
+        <v>75</v>
+      </c>
+      <c r="B63">
+        <v>2500</v>
+      </c>
+      <c r="C63">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D63">
+        <v>0.9</v>
+      </c>
+      <c r="E63" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" t="s">
+        <v>76</v>
+      </c>
+      <c r="B64">
+        <v>2500</v>
+      </c>
+      <c r="C64">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D64">
+        <v>0.9</v>
+      </c>
+      <c r="E64" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" t="s">
+        <v>77</v>
+      </c>
+      <c r="B65">
+        <v>2500</v>
+      </c>
+      <c r="C65">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D65">
+        <v>0.9</v>
+      </c>
+      <c r="E65" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" t="s">
+        <v>78</v>
+      </c>
+      <c r="B66">
+        <v>2500</v>
+      </c>
+      <c r="C66">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D66">
+        <v>0.9</v>
+      </c>
+      <c r="E66" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" t="s">
+        <v>79</v>
+      </c>
+      <c r="B67">
+        <v>2500</v>
+      </c>
+      <c r="C67">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D67">
+        <v>0.9</v>
+      </c>
+      <c r="E67" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" t="s">
+        <v>80</v>
+      </c>
+      <c r="B68">
+        <v>2500</v>
+      </c>
+      <c r="C68">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D68">
+        <v>0.9</v>
+      </c>
+      <c r="E68" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" t="s">
+        <v>81</v>
+      </c>
+      <c r="B69">
+        <v>2500</v>
+      </c>
+      <c r="C69">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D69">
+        <v>0.9</v>
+      </c>
+      <c r="E69" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" t="s">
+        <v>82</v>
+      </c>
+      <c r="B70">
+        <v>2500</v>
+      </c>
+      <c r="C70">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D70">
+        <v>0.9</v>
+      </c>
+      <c r="E70" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" t="s">
+        <v>83</v>
+      </c>
+      <c r="B71">
+        <v>2500</v>
+      </c>
+      <c r="C71">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D71">
+        <v>0.9</v>
+      </c>
+      <c r="E71" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" t="s">
+        <v>84</v>
+      </c>
+      <c r="B72">
+        <v>2500</v>
+      </c>
+      <c r="C72">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D72">
+        <v>0.9</v>
+      </c>
+      <c r="E72" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" t="s">
+        <v>85</v>
+      </c>
+      <c r="B73">
+        <v>2500</v>
+      </c>
+      <c r="C73">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D73">
+        <v>0.9</v>
+      </c>
+      <c r="E73" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" t="s">
+        <v>86</v>
+      </c>
+      <c r="B74">
+        <v>2500</v>
+      </c>
+      <c r="C74">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D74">
+        <v>0.9</v>
+      </c>
+      <c r="E74" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" t="s">
+        <v>87</v>
+      </c>
+      <c r="B75">
+        <v>2500</v>
+      </c>
+      <c r="C75">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D75">
+        <v>0.9</v>
+      </c>
+      <c r="E75" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" t="s">
+        <v>88</v>
+      </c>
+      <c r="B76">
+        <v>2500</v>
+      </c>
+      <c r="C76">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D76">
+        <v>0.9</v>
+      </c>
+      <c r="E76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" t="s">
+        <v>89</v>
+      </c>
+      <c r="B77">
+        <v>2500</v>
+      </c>
+      <c r="C77">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D77">
+        <v>0.9</v>
+      </c>
+      <c r="E77" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78" t="s">
+        <v>90</v>
+      </c>
+      <c r="B78">
+        <v>2500</v>
+      </c>
+      <c r="C78">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D78">
+        <v>0.9</v>
+      </c>
+      <c r="E78" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79" t="s">
+        <v>91</v>
+      </c>
+      <c r="B79">
+        <v>2500</v>
+      </c>
+      <c r="C79">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D79">
+        <v>0.9</v>
+      </c>
+      <c r="E79" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80" t="s">
+        <v>92</v>
+      </c>
+      <c r="B80">
+        <v>2500</v>
+      </c>
+      <c r="C80">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D80">
+        <v>0.9</v>
+      </c>
+      <c r="E80" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81" t="s">
+        <v>93</v>
+      </c>
+      <c r="B81">
+        <v>2500</v>
+      </c>
+      <c r="C81">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D81">
+        <v>0.9</v>
+      </c>
+      <c r="E81" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="A82" t="s">
+        <v>94</v>
+      </c>
+      <c r="B82">
+        <v>2500</v>
+      </c>
+      <c r="C82">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D82">
+        <v>0.9</v>
+      </c>
+      <c r="E82" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
+      <c r="A83" t="s">
+        <v>95</v>
+      </c>
+      <c r="B83">
+        <v>2500</v>
+      </c>
+      <c r="C83">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D83">
+        <v>0.9</v>
+      </c>
+      <c r="E83" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
+      <c r="A84" t="s">
+        <v>96</v>
+      </c>
+      <c r="B84">
+        <v>2500</v>
+      </c>
+      <c r="C84">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D84">
+        <v>0.9</v>
+      </c>
+      <c r="E84" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
+      <c r="A85" t="s">
+        <v>97</v>
+      </c>
+      <c r="B85">
+        <v>2500</v>
+      </c>
+      <c r="C85">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D85">
+        <v>0.9</v>
+      </c>
+      <c r="E85" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -708,7 +2154,7 @@
       <selection activeCell="B3" sqref="B3:D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15.25"/>
   <sheetData>
     <row r="3" spans="2:4">
       <c r="B3" t="s">

</xml_diff>

<commit_message>
More details for HotelLarge.idf
</commit_message>
<xml_diff>
--- a/data/material.xlsx
+++ b/data/material.xlsx
@@ -1,21 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sahina\PycharmProjects\Kamila\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/n/code/BuildME/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A12EEDEB-AFE0-4BA9-9ACA-8ED29460F6A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{631B7836-D1C9-2F47-8896-BDCE5DF464FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="95880" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{F14F42AE-B2B5-F34E-80E7-10F24B944563}"/>
+    <workbookView xWindow="-2680" yWindow="-26860" windowWidth="34560" windowHeight="21580" xr2:uid="{F14F42AE-B2B5-F34E-80E7-10F24B944563}"/>
   </bookViews>
   <sheets>
     <sheet name="properties" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">properties!$A$1:$E$83</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24,9 +27,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="96">
   <si>
     <t>Bldg_paper_felt</t>
   </si>
@@ -112,21 +113,9 @@
     <t>ext_blind</t>
   </si>
   <si>
-    <t>Opaque Door panel_con-efficient-RES0</t>
-  </si>
-  <si>
     <t>USA</t>
   </si>
   <si>
-    <t>Overhead Door_con Panel-efficient-RES0</t>
-  </si>
-  <si>
-    <t>CP02 CARPET PAD-efficient-RES0</t>
-  </si>
-  <si>
-    <t>Air_Wall_Material-efficient-RES0</t>
-  </si>
-  <si>
     <t>Nonres_Roof_Insulation-efficient-RES0</t>
   </si>
   <si>
@@ -154,21 +143,9 @@
     <t>Semiheated_Floor_Insulation-efficient-RES0</t>
   </si>
   <si>
-    <t>Std Opaque Door Panel-efficient-RES0</t>
-  </si>
-  <si>
-    <t>Opaque Door panel_con-non-standard-RES0</t>
-  </si>
-  <si>
     <t>Overhead Door_con Panel-non-standard-RES0</t>
   </si>
   <si>
-    <t>CP02 CARPET PAD-non-standard-RES0</t>
-  </si>
-  <si>
-    <t>Air_Wall_Material-non-standard-RES0</t>
-  </si>
-  <si>
     <t>Nonres_Roof_Insulation-non-standard-RES0</t>
   </si>
   <si>
@@ -196,21 +173,9 @@
     <t>Semiheated_Floor_Insulation-non-standard-RES0</t>
   </si>
   <si>
-    <t>Std Opaque Door Panel-non-standard-RES0</t>
-  </si>
-  <si>
-    <t>Opaque Door panel_con-standard-RES0</t>
-  </si>
-  <si>
     <t>Overhead Door_con Panel-standard-RES0</t>
   </si>
   <si>
-    <t>CP02 CARPET PAD-standard-RES0</t>
-  </si>
-  <si>
-    <t>Air_Wall_Material-standard-RES0</t>
-  </si>
-  <si>
     <t>Nonres_Roof_Insulation-standard-RES0</t>
   </si>
   <si>
@@ -238,21 +203,9 @@
     <t>Semiheated_Floor_Insulation-standard-RES0</t>
   </si>
   <si>
-    <t>Std Opaque Door Panel-standard-RES0</t>
-  </si>
-  <si>
-    <t>Opaque Door panel_con-ZEB-RES0</t>
-  </si>
-  <si>
     <t>Overhead Door_con Panel-ZEB-RES0</t>
   </si>
   <si>
-    <t>CP02 CARPET PAD-ZEB-RES0</t>
-  </si>
-  <si>
-    <t>Air_Wall_Material-ZEB-RES0</t>
-  </si>
-  <si>
     <t>Nonres_Roof_Insulation-ZEB-RES0</t>
   </si>
   <si>
@@ -280,9 +233,6 @@
     <t>Semiheated_Floor_Insulation-ZEB-RES0</t>
   </si>
   <si>
-    <t>Std Opaque Door Panel-ZEB-RES0</t>
-  </si>
-  <si>
     <t>Glazing Layer-efficient-RES0</t>
   </si>
   <si>
@@ -329,6 +279,51 @@
   </si>
   <si>
     <t>Nonres Skylight Glazing Layer-ZEB-RES0</t>
+  </si>
+  <si>
+    <t>Opaque Door panel_con-efficient</t>
+  </si>
+  <si>
+    <t>Overhead Door_con Panel-efficient</t>
+  </si>
+  <si>
+    <t>CP02 CARPET PAD-efficient</t>
+  </si>
+  <si>
+    <t>Std Opaque Door Panel-efficient</t>
+  </si>
+  <si>
+    <t>Std Opaque Door Panel-non-standard</t>
+  </si>
+  <si>
+    <t>Std Opaque Door Panel-standard</t>
+  </si>
+  <si>
+    <t>Std Opaque Door Panel-ZEB</t>
+  </si>
+  <si>
+    <t>CP02 CARPET PAD-ZEB</t>
+  </si>
+  <si>
+    <t>CP02 CARPET PAD-non-standard</t>
+  </si>
+  <si>
+    <t>CP02 CARPET PAD-standard</t>
+  </si>
+  <si>
+    <t>CP02 CARPET PAD</t>
+  </si>
+  <si>
+    <t>Opaque Door panel_con-non-standard</t>
+  </si>
+  <si>
+    <t>Opaque Door panel_con-standard</t>
+  </si>
+  <si>
+    <t>Opaque Door panel_con-ZEB</t>
+  </si>
+  <si>
+    <t>Air_Wall_Material</t>
   </si>
 </sst>
 </file>
@@ -378,11 +373,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -697,19 +693,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E70C4D75-A999-1F4A-8C48-1C4FDC3CB665}">
-  <dimension ref="A1:E85"/>
+  <dimension ref="A1:E83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A69" sqref="A69"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3:XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="47.0703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="47" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.5">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -728,265 +725,265 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B2">
-        <v>575</v>
+        <v>1.2</v>
       </c>
       <c r="C2">
-        <v>1.2999999999999999E-4</v>
+        <v>0.1</v>
       </c>
       <c r="D2">
-        <v>0.2</v>
+        <v>0.63</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>95</v>
       </c>
       <c r="B3">
-        <v>100</v>
+        <v>2500</v>
       </c>
       <c r="C3">
-        <v>0.1</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="D3">
-        <v>0.04</v>
+        <v>0.9</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B4">
-        <v>1.2</v>
+        <v>575</v>
       </c>
       <c r="C4">
-        <v>0.1</v>
+        <v>1.2999999999999999E-4</v>
       </c>
       <c r="D4">
-        <v>0.63</v>
+        <v>0.2</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="15.5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>2500</v>
-      </c>
-      <c r="C5">
+        <v>1050</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B6">
+        <v>2500</v>
+      </c>
+      <c r="C6">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D6">
+        <v>0.9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B7">
+        <v>2500</v>
+      </c>
+      <c r="C7">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D7">
+        <v>0.9</v>
+      </c>
+      <c r="E7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B8">
+        <v>2500</v>
+      </c>
+      <c r="C8">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D8">
+        <v>0.9</v>
+      </c>
+      <c r="E8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>90</v>
+      </c>
+      <c r="B9">
+        <v>2500</v>
+      </c>
+      <c r="C9">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D9">
+        <v>0.9</v>
+      </c>
+      <c r="E9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B10">
+        <v>2500</v>
+      </c>
+      <c r="C10">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D10">
+        <v>0.9</v>
+      </c>
+      <c r="E10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11">
+        <v>1050</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14">
+        <v>2500</v>
+      </c>
+      <c r="C14">
         <f>2*0.004</f>
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.5">
-      <c r="A6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6">
-        <v>2500</v>
-      </c>
-      <c r="C6">
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15">
+        <v>2500</v>
+      </c>
+      <c r="C15">
         <f>2*0.004</f>
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.5">
-      <c r="A7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7">
-        <v>2500</v>
-      </c>
-      <c r="C7">
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16">
+        <v>2500</v>
+      </c>
+      <c r="C16">
         <f>2*0.004</f>
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.5">
-      <c r="A8" t="s">
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
         <v>22</v>
       </c>
-      <c r="B8">
-        <v>2500</v>
-      </c>
-      <c r="C8">
+      <c r="B17">
+        <v>2500</v>
+      </c>
+      <c r="C17">
         <f>2*0.004</f>
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="15.5">
-      <c r="A10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10">
-        <v>1050</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="15.5">
-      <c r="A11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11">
-        <v>1050</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14">
-        <v>2500</v>
-      </c>
-      <c r="C14">
-        <v>6.0000000000000001E-3</v>
-      </c>
-      <c r="D14">
-        <v>0.9</v>
-      </c>
-      <c r="E14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15">
-        <v>2500</v>
-      </c>
-      <c r="C15">
-        <v>6.0000000000000001E-3</v>
-      </c>
-      <c r="D15">
-        <v>0.9</v>
-      </c>
-      <c r="E15" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16">
-        <v>2500</v>
-      </c>
-      <c r="C16">
-        <v>6.0000000000000001E-3</v>
-      </c>
-      <c r="D16">
-        <v>0.9</v>
-      </c>
-      <c r="E16" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17">
-        <v>2500</v>
-      </c>
-      <c r="C17">
-        <v>6.0000000000000001E-3</v>
-      </c>
-      <c r="D17">
-        <v>0.9</v>
-      </c>
-      <c r="E17" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>30</v>
+        <v>65</v>
       </c>
       <c r="B18">
         <v>2500</v>
@@ -998,12 +995,12 @@
         <v>0.9</v>
       </c>
       <c r="E18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>31</v>
+        <v>67</v>
       </c>
       <c r="B19">
         <v>2500</v>
@@ -1015,12 +1012,12 @@
         <v>0.9</v>
       </c>
       <c r="E19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>32</v>
+        <v>69</v>
       </c>
       <c r="B20">
         <v>2500</v>
@@ -1032,12 +1029,12 @@
         <v>0.9</v>
       </c>
       <c r="E20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>33</v>
+        <v>71</v>
       </c>
       <c r="B21">
         <v>2500</v>
@@ -1049,29 +1046,29 @@
         <v>0.9</v>
       </c>
       <c r="E21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="B22">
-        <v>2500</v>
+        <v>0</v>
       </c>
       <c r="C22">
-        <v>6.0000000000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="D22">
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="E22" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>35</v>
+        <v>74</v>
       </c>
       <c r="B23">
         <v>2500</v>
@@ -1083,12 +1080,12 @@
         <v>0.9</v>
       </c>
       <c r="E23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>36</v>
+        <v>76</v>
       </c>
       <c r="B24">
         <v>2500</v>
@@ -1100,12 +1097,12 @@
         <v>0.9</v>
       </c>
       <c r="E24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>37</v>
+        <v>78</v>
       </c>
       <c r="B25">
         <v>2500</v>
@@ -1117,12 +1114,12 @@
         <v>0.9</v>
       </c>
       <c r="E25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>38</v>
+        <v>80</v>
       </c>
       <c r="B26">
         <v>2500</v>
@@ -1134,12 +1131,12 @@
         <v>0.9</v>
       </c>
       <c r="E26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>39</v>
+        <v>73</v>
       </c>
       <c r="B27">
         <v>2500</v>
@@ -1151,12 +1148,12 @@
         <v>0.9</v>
       </c>
       <c r="E27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>40</v>
+        <v>75</v>
       </c>
       <c r="B28">
         <v>2500</v>
@@ -1168,12 +1165,12 @@
         <v>0.9</v>
       </c>
       <c r="E28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>41</v>
+        <v>77</v>
       </c>
       <c r="B29">
         <v>2500</v>
@@ -1185,12 +1182,12 @@
         <v>0.9</v>
       </c>
       <c r="E29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" t="s">
-        <v>42</v>
+        <v>79</v>
       </c>
       <c r="B30">
         <v>2500</v>
@@ -1202,12 +1199,12 @@
         <v>0.9</v>
       </c>
       <c r="E30" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="B31">
         <v>2500</v>
@@ -1219,12 +1216,12 @@
         <v>0.9</v>
       </c>
       <c r="E31" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B32">
         <v>2500</v>
@@ -1236,12 +1233,12 @@
         <v>0.9</v>
       </c>
       <c r="E32" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B33">
         <v>2500</v>
@@ -1253,12 +1250,12 @@
         <v>0.9</v>
       </c>
       <c r="E33" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="B34">
         <v>2500</v>
@@ -1270,12 +1267,12 @@
         <v>0.9</v>
       </c>
       <c r="E34" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="B35">
         <v>2500</v>
@@ -1287,12 +1284,12 @@
         <v>0.9</v>
       </c>
       <c r="E35" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B36">
         <v>2500</v>
@@ -1304,12 +1301,12 @@
         <v>0.9</v>
       </c>
       <c r="E36" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B37">
         <v>2500</v>
@@ -1321,12 +1318,12 @@
         <v>0.9</v>
       </c>
       <c r="E37" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="B38">
         <v>2500</v>
@@ -1338,12 +1335,12 @@
         <v>0.9</v>
       </c>
       <c r="E38" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="B39">
         <v>2500</v>
@@ -1355,12 +1352,12 @@
         <v>0.9</v>
       </c>
       <c r="E39" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="B40">
         <v>2500</v>
@@ -1372,12 +1369,12 @@
         <v>0.9</v>
       </c>
       <c r="E40" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B41">
         <v>2500</v>
@@ -1389,12 +1386,12 @@
         <v>0.9</v>
       </c>
       <c r="E41" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B42">
         <v>2500</v>
@@ -1406,12 +1403,12 @@
         <v>0.9</v>
       </c>
       <c r="E42" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" t="s">
-        <v>55</v>
+        <v>81</v>
       </c>
       <c r="B43">
         <v>2500</v>
@@ -1423,12 +1420,12 @@
         <v>0.9</v>
       </c>
       <c r="E43" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" t="s">
-        <v>56</v>
+        <v>92</v>
       </c>
       <c r="B44">
         <v>2500</v>
@@ -1440,12 +1437,12 @@
         <v>0.9</v>
       </c>
       <c r="E44" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" t="s">
-        <v>57</v>
+        <v>93</v>
       </c>
       <c r="B45">
         <v>2500</v>
@@ -1457,12 +1454,12 @@
         <v>0.9</v>
       </c>
       <c r="E45" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" t="s">
-        <v>58</v>
+        <v>94</v>
       </c>
       <c r="B46">
         <v>2500</v>
@@ -1474,12 +1471,12 @@
         <v>0.9</v>
       </c>
       <c r="E46" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" t="s">
-        <v>59</v>
+        <v>82</v>
       </c>
       <c r="B47">
         <v>2500</v>
@@ -1491,12 +1488,12 @@
         <v>0.9</v>
       </c>
       <c r="E47" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="B48">
         <v>2500</v>
@@ -1508,12 +1505,12 @@
         <v>0.9</v>
       </c>
       <c r="E48" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="B49">
         <v>2500</v>
@@ -1525,12 +1522,12 @@
         <v>0.9</v>
       </c>
       <c r="E49" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="B50">
         <v>2500</v>
@@ -1542,29 +1539,29 @@
         <v>0.9</v>
       </c>
       <c r="E50" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" t="s">
-        <v>63</v>
+        <v>1</v>
       </c>
       <c r="B51">
-        <v>2500</v>
+        <v>100</v>
       </c>
       <c r="C51">
-        <v>6.0000000000000001E-3</v>
+        <v>0.1</v>
       </c>
       <c r="D51">
-        <v>0.9</v>
+        <v>0.04</v>
       </c>
       <c r="E51" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" t="s">
-        <v>64</v>
+        <v>30</v>
       </c>
       <c r="B52">
         <v>2500</v>
@@ -1576,12 +1573,12 @@
         <v>0.9</v>
       </c>
       <c r="E52" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="B53">
         <v>2500</v>
@@ -1593,12 +1590,12 @@
         <v>0.9</v>
       </c>
       <c r="E53" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="B54">
         <v>2500</v>
@@ -1610,12 +1607,12 @@
         <v>0.9</v>
       </c>
       <c r="E54" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B55">
         <v>2500</v>
@@ -1627,12 +1624,12 @@
         <v>0.9</v>
       </c>
       <c r="E55" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" t="s">
-        <v>68</v>
+        <v>33</v>
       </c>
       <c r="B56">
         <v>2500</v>
@@ -1644,12 +1641,12 @@
         <v>0.9</v>
       </c>
       <c r="E56" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" t="s">
-        <v>69</v>
+        <v>43</v>
       </c>
       <c r="B57">
         <v>2500</v>
@@ -1661,12 +1658,12 @@
         <v>0.9</v>
       </c>
       <c r="E57" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="B58">
         <v>2500</v>
@@ -1678,12 +1675,12 @@
         <v>0.9</v>
       </c>
       <c r="E58" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="59" spans="1:5">
       <c r="A59" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B59">
         <v>2500</v>
@@ -1695,12 +1692,12 @@
         <v>0.9</v>
       </c>
       <c r="E59" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" t="s">
-        <v>72</v>
+        <v>27</v>
       </c>
       <c r="B60">
         <v>2500</v>
@@ -1712,12 +1709,12 @@
         <v>0.9</v>
       </c>
       <c r="E60" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="61" spans="1:5">
       <c r="A61" t="s">
-        <v>73</v>
+        <v>37</v>
       </c>
       <c r="B61">
         <v>2500</v>
@@ -1729,12 +1726,12 @@
         <v>0.9</v>
       </c>
       <c r="E61" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="62" spans="1:5">
       <c r="A62" t="s">
-        <v>74</v>
+        <v>47</v>
       </c>
       <c r="B62">
         <v>2500</v>
@@ -1746,12 +1743,12 @@
         <v>0.9</v>
       </c>
       <c r="E62" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="63" spans="1:5">
       <c r="A63" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="B63">
         <v>2500</v>
@@ -1763,12 +1760,12 @@
         <v>0.9</v>
       </c>
       <c r="E63" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="64" spans="1:5">
       <c r="A64" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="B64">
         <v>2500</v>
@@ -1780,12 +1777,12 @@
         <v>0.9</v>
       </c>
       <c r="E64" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="65" spans="1:5">
       <c r="A65" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="B65">
         <v>2500</v>
@@ -1797,12 +1794,12 @@
         <v>0.9</v>
       </c>
       <c r="E65" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="66" spans="1:5">
       <c r="A66" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="B66">
         <v>2500</v>
@@ -1814,12 +1811,12 @@
         <v>0.9</v>
       </c>
       <c r="E66" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="67" spans="1:5">
       <c r="A67" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="B67">
         <v>2500</v>
@@ -1831,12 +1828,12 @@
         <v>0.9</v>
       </c>
       <c r="E67" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="68" spans="1:5">
       <c r="A68" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="B68">
         <v>2500</v>
@@ -1848,12 +1845,12 @@
         <v>0.9</v>
       </c>
       <c r="E68" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="69" spans="1:5">
       <c r="A69" t="s">
-        <v>81</v>
+        <v>41</v>
       </c>
       <c r="B69">
         <v>2500</v>
@@ -1865,12 +1862,12 @@
         <v>0.9</v>
       </c>
       <c r="E69" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="70" spans="1:5">
       <c r="A70" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
       <c r="B70">
         <v>2500</v>
@@ -1882,12 +1879,12 @@
         <v>0.9</v>
       </c>
       <c r="E70" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="71" spans="1:5">
       <c r="A71" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="B71">
         <v>2500</v>
@@ -1899,12 +1896,12 @@
         <v>0.9</v>
       </c>
       <c r="E71" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="72" spans="1:5">
       <c r="A72" t="s">
-        <v>84</v>
+        <v>34</v>
       </c>
       <c r="B72">
         <v>2500</v>
@@ -1916,12 +1913,12 @@
         <v>0.9</v>
       </c>
       <c r="E72" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="73" spans="1:5">
       <c r="A73" t="s">
-        <v>85</v>
+        <v>44</v>
       </c>
       <c r="B73">
         <v>2500</v>
@@ -1933,12 +1930,12 @@
         <v>0.9</v>
       </c>
       <c r="E73" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="74" spans="1:5">
       <c r="A74" t="s">
-        <v>86</v>
+        <v>54</v>
       </c>
       <c r="B74">
         <v>2500</v>
@@ -1950,12 +1947,12 @@
         <v>0.9</v>
       </c>
       <c r="E74" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="75" spans="1:5">
       <c r="A75" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
       <c r="B75">
         <v>2500</v>
@@ -1967,12 +1964,12 @@
         <v>0.9</v>
       </c>
       <c r="E75" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="76" spans="1:5">
       <c r="A76" t="s">
-        <v>88</v>
+        <v>28</v>
       </c>
       <c r="B76">
         <v>2500</v>
@@ -1984,12 +1981,12 @@
         <v>0.9</v>
       </c>
       <c r="E76" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="77" spans="1:5">
       <c r="A77" t="s">
-        <v>89</v>
+        <v>38</v>
       </c>
       <c r="B77">
         <v>2500</v>
@@ -2001,12 +1998,12 @@
         <v>0.9</v>
       </c>
       <c r="E77" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="78" spans="1:5">
       <c r="A78" t="s">
-        <v>90</v>
+        <v>48</v>
       </c>
       <c r="B78">
         <v>2500</v>
@@ -2018,12 +2015,12 @@
         <v>0.9</v>
       </c>
       <c r="E78" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="79" spans="1:5">
       <c r="A79" t="s">
-        <v>91</v>
+        <v>58</v>
       </c>
       <c r="B79">
         <v>2500</v>
@@ -2035,12 +2032,12 @@
         <v>0.9</v>
       </c>
       <c r="E79" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="80" spans="1:5">
       <c r="A80" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="B80">
         <v>2500</v>
@@ -2052,12 +2049,12 @@
         <v>0.9</v>
       </c>
       <c r="E80" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="81" spans="1:5">
       <c r="A81" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="B81">
         <v>2500</v>
@@ -2069,12 +2066,12 @@
         <v>0.9</v>
       </c>
       <c r="E81" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="82" spans="1:5">
-      <c r="A82" t="s">
-        <v>94</v>
+      <c r="A82" s="4" t="s">
+        <v>86</v>
       </c>
       <c r="B82">
         <v>2500</v>
@@ -2086,12 +2083,12 @@
         <v>0.9</v>
       </c>
       <c r="E82" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="83" spans="1:5">
       <c r="A83" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="B83">
         <v>2500</v>
@@ -2103,44 +2100,11 @@
         <v>0.9</v>
       </c>
       <c r="E83" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5">
-      <c r="A84" t="s">
-        <v>96</v>
-      </c>
-      <c r="B84">
-        <v>2500</v>
-      </c>
-      <c r="C84">
-        <v>6.0000000000000001E-3</v>
-      </c>
-      <c r="D84">
-        <v>0.9</v>
-      </c>
-      <c r="E84" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5">
-      <c r="A85" t="s">
-        <v>97</v>
-      </c>
-      <c r="B85">
-        <v>2500</v>
-      </c>
-      <c r="C85">
-        <v>6.0000000000000001E-3</v>
-      </c>
-      <c r="D85">
-        <v>0.9</v>
-      </c>
-      <c r="E85" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E83" xr:uid="{E70C4D75-A999-1F4A-8C48-1C4FDC3CB665}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
@@ -2154,7 +2118,7 @@
       <selection activeCell="B3" sqref="B3:D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="16"/>
   <sheetData>
     <row r="3" spans="2:4">
       <c r="B3" t="s">

</xml_diff>